<commit_message>
nit por linea preactivador
</commit_message>
<xml_diff>
--- a/src/preactivador/preactivador.xlsx
+++ b/src/preactivador/preactivador.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Olimpostudio\Temporales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250886FB-3672-4613-8355-0C4E404B45A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C9DFFC-D265-4CDB-AEAC-62944DA1C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <t>Mensaje</t>
   </si>
   <si>
-    <t>Error en activacion</t>
+    <t>Nit</t>
   </si>
 </sst>
 </file>
@@ -87,15 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,31 +394,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>